<commit_message>
Various problems from the last few months
</commit_message>
<xml_diff>
--- a/Spring 2018 Hours Log.xlsx
+++ b/Spring 2018 Hours Log.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertcabello/Documents/College/Programming Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58D7EEB-B374-C244-A616-20522D094728}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{CC9EF2E6-B1D8-4F4D-8995-2A81B177D8FC}"/>
+    <workbookView xWindow="760" yWindow="480" windowWidth="28040" windowHeight="15940" xr2:uid="{CC9EF2E6-B1D8-4F4D-8995-2A81B177D8FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +55,18 @@
   </si>
   <si>
     <t>Wednesday Session and practice with Jesus</t>
+  </si>
+  <si>
+    <t>Project Euler+ Problems on Hackerrank</t>
+  </si>
+  <si>
+    <t>Saturday Session with Jesus</t>
+  </si>
+  <si>
+    <t>Wednesday Session and Kattis Practice</t>
+  </si>
+  <si>
+    <t>High School Competition</t>
   </si>
 </sst>
 </file>
@@ -89,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAA7741-9206-A340-9CFA-F976C73BFEC7}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,11 +460,11 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <f>SUM($B$2:$B2)</f>
+        <f>SUM($B$2:B2)</f>
         <v>3</v>
       </c>
       <c r="E2">
-        <f>(15 * $D2)</f>
+        <f>15*D2</f>
         <v>45</v>
       </c>
     </row>
@@ -465,11 +479,11 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f>SUM($B$2:$B3)</f>
+        <f>SUM($B$2:B3)</f>
         <v>5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E15" si="0">(15 * $D3)</f>
+        <f t="shared" ref="E3:E22" si="0">15*D3</f>
         <v>75</v>
       </c>
     </row>
@@ -484,7 +498,7 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <f>SUM($B$2:$B4)</f>
+        <f>SUM($B$2:B4)</f>
         <v>6</v>
       </c>
       <c r="E4">
@@ -503,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <f>SUM($B$2:$B5)</f>
+        <f>SUM($B$2:B5)</f>
         <v>7</v>
       </c>
       <c r="E5">
@@ -522,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <f>SUM($B$2:$B6)</f>
+        <f>SUM($B$2:B6)</f>
         <v>10</v>
       </c>
       <c r="E6">
@@ -541,7 +555,7 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <f>SUM($B$2:$B7)</f>
+        <f>SUM($B$2:B7)</f>
         <v>10.5</v>
       </c>
       <c r="E7">
@@ -560,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <f>SUM($B$2:$B8)</f>
+        <f>SUM($B$2:B8)</f>
         <v>13.5</v>
       </c>
       <c r="E8">
@@ -579,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <f>SUM($B$2:$B9)</f>
+        <f>SUM($B$2:B9)</f>
         <v>15</v>
       </c>
       <c r="E9">
@@ -598,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <f>SUM($B$2:$B10)</f>
+        <f>SUM($B$2:B10)</f>
         <v>18</v>
       </c>
       <c r="E10">
@@ -607,59 +621,220 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43148</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
       <c r="D11">
-        <f>SUM($B$2:$B11)</f>
-        <v>18</v>
+        <f>SUM($B$2:B11)</f>
+        <v>21</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43152</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
       <c r="D12">
-        <f>SUM($B$2:$B12)</f>
-        <v>18</v>
+        <f>SUM($B$2:B12)</f>
+        <v>23</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43159</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
       <c r="D13">
-        <f>SUM($B$2:$B13)</f>
-        <v>18</v>
+        <f>SUM($B$2:B13)</f>
+        <v>25</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43166</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
       <c r="D14">
-        <f>SUM($B$2:$B14)</f>
-        <v>18</v>
+        <f>SUM($B$2:B14)</f>
+        <v>27</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43176</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
       <c r="D15">
-        <f>SUM($B$2:$B15)</f>
-        <v>18</v>
+        <f>SUM($B$2:B15)</f>
+        <v>29</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43180</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <f>SUM($B$2:B16)</f>
+        <v>33</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>43190</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <f>SUM($B$2:B17)</f>
+        <v>35</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43197</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <f>SUM($B$2:B18)</f>
+        <v>37</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>555</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43201</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <f>SUM($B$2:B19)</f>
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43204</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <f>SUM($B$2:B20)</f>
+        <v>47</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f>SUM($B$2:B21)</f>
+        <v>47</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f>SUM($B$2:B22)</f>
+        <v>47</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>705</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="D3" formulaRange="1"/>
+    <ignoredError sqref="D3:D16" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>